<commit_message>
Actualización de escaleta guion 5
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Escaleta_LE_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Escaleta_LE_08_05_CO.xlsx
@@ -909,9 +909,6 @@
     <t>Recurso M101A-04</t>
   </si>
   <si>
-    <t>Recurso M101A-05</t>
-  </si>
-  <si>
     <t>Recurso F6B-01</t>
   </si>
   <si>
@@ -1000,6 +997,9 @@
   </si>
   <si>
     <t xml:space="preserve">A partir de la observación de un video, los estudiantes deben ordenar oraciones simples de acuerdo a la secuencia de este. Video titulado El Anarquismo. Tomado de: CS_10_04, La sociedad industrial y sus ideologías, El anarquismo, CIENCIAS SOCIALES, GEOGRAFÍA E HISTORIA. </t>
+  </si>
+  <si>
+    <t>Recurso M4A-01</t>
   </si>
 </sst>
 </file>
@@ -1322,6 +1322,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1332,12 +1359,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1378,27 +1399,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1706,9 +1706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1737,94 +1737,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="17" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="51" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="P1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="70" t="s">
+      <c r="R1" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="66" t="s">
+      <c r="S1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="68" t="s">
+      <c r="T1" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="66" t="s">
+      <c r="U1" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="65"/>
       <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="67"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1864,7 +1864,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>19</v>
@@ -1878,7 +1878,7 @@
       <c r="S3" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T3" s="72" t="s">
+      <c r="T3" s="47" t="s">
         <v>265</v>
       </c>
       <c r="U3" s="34" t="s">
@@ -1937,7 +1937,7 @@
       <c r="S4" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T4" s="72" t="s">
+      <c r="T4" s="47" t="s">
         <v>267</v>
       </c>
       <c r="U4" s="34" t="s">
@@ -1982,7 +1982,7 @@
         <v>49</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>19</v>
@@ -1996,7 +1996,7 @@
       <c r="S5" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T5" s="72" t="s">
+      <c r="T5" s="47" t="s">
         <v>268</v>
       </c>
       <c r="U5" s="34" t="s">
@@ -2019,7 +2019,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="23"/>
       <c r="G6" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H6" s="38">
         <v>4</v>
@@ -2041,7 +2041,7 @@
         <v>27</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>19</v>
@@ -2055,7 +2055,7 @@
       <c r="S6" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T6" s="72" t="s">
+      <c r="T6" s="47" t="s">
         <v>269</v>
       </c>
       <c r="U6" s="34" t="s">
@@ -2114,7 +2114,7 @@
       <c r="S7" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T7" s="72" t="s">
+      <c r="T7" s="47" t="s">
         <v>270</v>
       </c>
       <c r="U7" s="34" t="s">
@@ -2159,7 +2159,7 @@
         <v>120</v>
       </c>
       <c r="O8" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P8" s="24" t="s">
         <v>19</v>
@@ -2173,7 +2173,7 @@
       <c r="S8" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T8" s="72" t="s">
+      <c r="T8" s="47" t="s">
         <v>271</v>
       </c>
       <c r="U8" s="34" t="s">
@@ -2236,7 +2236,7 @@
       <c r="S9" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T9" s="72" t="s">
+      <c r="T9" s="47" t="s">
         <v>272</v>
       </c>
       <c r="U9" s="34" t="s">
@@ -2285,7 +2285,7 @@
         <v>28</v>
       </c>
       <c r="O10" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P10" s="24" t="s">
         <v>19</v>
@@ -2299,7 +2299,7 @@
       <c r="S10" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T10" s="72" t="s">
+      <c r="T10" s="47" t="s">
         <v>273</v>
       </c>
       <c r="U10" s="34" t="s">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P11" s="24" t="s">
         <v>19</v>
@@ -2362,7 +2362,7 @@
       <c r="S11" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="T11" s="72" t="s">
+      <c r="T11" s="47" t="s">
         <v>276</v>
       </c>
       <c r="U11" s="34" t="s">
@@ -2398,7 +2398,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>20</v>
@@ -2425,7 +2425,7 @@
       <c r="S12" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T12" s="72" t="s">
+      <c r="T12" s="47" t="s">
         <v>278</v>
       </c>
       <c r="U12" s="34" t="s">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P13" s="24" t="s">
         <v>19</v>
@@ -2488,7 +2488,7 @@
       <c r="S13" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="T13" s="72" t="s">
+      <c r="T13" s="47" t="s">
         <v>279</v>
       </c>
       <c r="U13" s="34" t="s">
@@ -2537,7 +2537,7 @@
         <v>44</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P14" s="24" t="s">
         <v>20</v>
@@ -2551,7 +2551,7 @@
       <c r="S14" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T14" s="72" t="s">
+      <c r="T14" s="47" t="s">
         <v>280</v>
       </c>
       <c r="U14" s="34" t="s">
@@ -2612,7 +2612,7 @@
       <c r="S15" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T15" s="72" t="s">
+      <c r="T15" s="47" t="s">
         <v>281</v>
       </c>
       <c r="U15" s="34" t="s">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P16" s="24" t="s">
         <v>19</v>
@@ -2673,8 +2673,8 @@
       <c r="S16" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="T16" s="72" t="s">
-        <v>285</v>
+      <c r="T16" s="47" t="s">
+        <v>284</v>
       </c>
       <c r="U16" s="34" t="s">
         <v>277</v>
@@ -2732,7 +2732,7 @@
       <c r="S17" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="T17" s="72" t="s">
+      <c r="T17" s="47" t="s">
         <v>144</v>
       </c>
       <c r="U17" s="34" t="s">
@@ -2791,7 +2791,7 @@
       <c r="S18" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="T18" s="72" t="s">
+      <c r="T18" s="47" t="s">
         <v>150</v>
       </c>
       <c r="U18" s="34" t="s">
@@ -2850,7 +2850,7 @@
       <c r="S19" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="T19" s="72" t="s">
+      <c r="T19" s="47" t="s">
         <v>152</v>
       </c>
       <c r="U19" s="34" t="s">
@@ -2909,7 +2909,7 @@
       <c r="S20" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="T20" s="72" t="s">
+      <c r="T20" s="47" t="s">
         <v>148</v>
       </c>
       <c r="U20" s="34" t="s">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H21" s="24">
         <v>19</v>
@@ -2968,7 +2968,7 @@
       <c r="S21" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="T21" s="72" t="s">
+      <c r="T21" s="47" t="s">
         <v>147</v>
       </c>
       <c r="U21" s="34" t="s">
@@ -3025,7 +3025,7 @@
       <c r="S22" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="T22" s="72" t="s">
+      <c r="T22" s="47" t="s">
         <v>168</v>
       </c>
       <c r="U22" s="34" t="s">
@@ -3082,7 +3082,7 @@
       <c r="S23" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="T23" s="72" t="s">
+      <c r="T23" s="47" t="s">
         <v>153</v>
       </c>
       <c r="U23" s="34" t="s">
@@ -3139,7 +3139,7 @@
       <c r="S24" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="T24" s="72" t="s">
+      <c r="T24" s="47" t="s">
         <v>159</v>
       </c>
       <c r="U24" s="34" t="s">
@@ -3171,7 +3171,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>19</v>
@@ -3196,7 +3196,7 @@
       <c r="S25" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="T25" s="72" t="s">
+      <c r="T25" s="47" t="s">
         <v>162</v>
       </c>
       <c r="U25" s="34" t="s">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H26" s="24">
         <v>24</v>
@@ -3243,7 +3243,7 @@
         <v>120</v>
       </c>
       <c r="O26" s="43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P26" s="24" t="s">
         <v>19</v>
@@ -3257,7 +3257,7 @@
       <c r="S26" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="T26" s="72" t="s">
+      <c r="T26" s="47" t="s">
         <v>166</v>
       </c>
       <c r="U26" s="34" t="s">
@@ -3318,7 +3318,7 @@
       <c r="S27" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="T27" s="72" t="s">
+      <c r="T27" s="47" t="s">
         <v>173</v>
       </c>
       <c r="U27" s="34" t="s">
@@ -3379,8 +3379,8 @@
       <c r="S28" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T28" s="72" t="s">
-        <v>286</v>
+      <c r="T28" s="47" t="s">
+        <v>285</v>
       </c>
       <c r="U28" s="34" t="s">
         <v>266</v>
@@ -3440,8 +3440,8 @@
       <c r="S29" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T29" s="72" t="s">
-        <v>287</v>
+      <c r="T29" s="47" t="s">
+        <v>286</v>
       </c>
       <c r="U29" s="34" t="s">
         <v>266</v>
@@ -3501,7 +3501,7 @@
       <c r="S30" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T30" s="72" t="s">
+      <c r="T30" s="47" t="s">
         <v>282</v>
       </c>
       <c r="U30" s="34" t="s">
@@ -3562,8 +3562,8 @@
       <c r="S31" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T31" s="72" t="s">
-        <v>288</v>
+      <c r="T31" s="47" t="s">
+        <v>287</v>
       </c>
       <c r="U31" s="34" t="s">
         <v>266</v>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="N32" s="6"/>
       <c r="O32" s="23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P32" s="24" t="s">
         <v>19</v>
@@ -3623,7 +3623,7 @@
       <c r="S32" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="T32" s="72" t="s">
+      <c r="T32" s="47" t="s">
         <v>177</v>
       </c>
       <c r="U32" s="34" t="s">
@@ -3670,7 +3670,7 @@
         <v>120</v>
       </c>
       <c r="O33" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P33" s="24" t="s">
         <v>19</v>
@@ -3684,7 +3684,7 @@
       <c r="S33" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T33" s="72" t="s">
+      <c r="T33" s="47" t="s">
         <v>283</v>
       </c>
       <c r="U33" s="34" t="s">
@@ -3716,7 +3716,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>20</v>
@@ -3743,8 +3743,8 @@
       <c r="S34" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T34" s="72" t="s">
-        <v>289</v>
+      <c r="T34" s="47" t="s">
+        <v>288</v>
       </c>
       <c r="U34" s="34" t="s">
         <v>266</v>
@@ -3775,7 +3775,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>20</v>
@@ -3788,7 +3788,7 @@
         <v>47</v>
       </c>
       <c r="O35" s="23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P35" s="24" t="s">
         <v>19</v>
@@ -3802,8 +3802,8 @@
       <c r="S35" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T35" s="72" t="s">
-        <v>290</v>
+      <c r="T35" s="47" t="s">
+        <v>289</v>
       </c>
       <c r="U35" s="34" t="s">
         <v>266</v>
@@ -3861,8 +3861,8 @@
       <c r="S36" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T36" s="72" t="s">
-        <v>291</v>
+      <c r="T36" s="47" t="s">
+        <v>290</v>
       </c>
       <c r="U36" s="34" t="s">
         <v>266</v>
@@ -3920,8 +3920,8 @@
       <c r="S37" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T37" s="72" t="s">
-        <v>292</v>
+      <c r="T37" s="47" t="s">
+        <v>291</v>
       </c>
       <c r="U37" s="34" t="s">
         <v>266</v>
@@ -3979,8 +3979,8 @@
       <c r="S38" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T38" s="72" t="s">
-        <v>293</v>
+      <c r="T38" s="47" t="s">
+        <v>292</v>
       </c>
       <c r="U38" s="34" t="s">
         <v>266</v>
@@ -4026,7 +4026,7 @@
       <c r="Q39" s="34"/>
       <c r="R39" s="35"/>
       <c r="S39" s="36"/>
-      <c r="T39" s="72"/>
+      <c r="T39" s="47"/>
       <c r="U39" s="34"/>
     </row>
     <row r="40" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4064,7 +4064,7 @@
       </c>
       <c r="M40" s="6"/>
       <c r="N40" s="6" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="O40" s="23" t="s">
         <v>257</v>
@@ -4081,8 +4081,8 @@
       <c r="S40" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T40" s="72" t="s">
-        <v>284</v>
+      <c r="T40" s="47" t="s">
+        <v>314</v>
       </c>
       <c r="U40" s="34" t="s">
         <v>266</v>
@@ -4140,8 +4140,8 @@
       <c r="S41" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="T41" s="72" t="s">
-        <v>294</v>
+      <c r="T41" s="47" t="s">
+        <v>293</v>
       </c>
       <c r="U41" s="34" t="s">
         <v>266</v>
@@ -6141,12 +6141,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6161,6 +6155,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>